<commit_message>
Edits made to main.py on 10.30.23
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hgarrison/Library/CloudStorage/Egnyte-artiasolutions/Shared/Analytics/Staff/hgarrison/Database Project/Artia-Database/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608B997C-58A0-C848-87F9-D90EB38C0FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="4480" windowWidth="24980" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Util Sum" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="92">
   <si>
     <t>FFSU</t>
   </si>
@@ -254,6 +248,42 @@
   </si>
   <si>
     <t>Total Amount</t>
+  </si>
+  <si>
+    <t>WAC/Unit</t>
+  </si>
+  <si>
+    <t>NADAC/Unit</t>
+  </si>
+  <si>
+    <t>Est. URA</t>
+  </si>
+  <si>
+    <t>FUL</t>
+  </si>
+  <si>
+    <t>WAMP</t>
+  </si>
+  <si>
+    <t>Total WAC</t>
+  </si>
+  <si>
+    <t>Total Pharmacy Reimbursement</t>
+  </si>
+  <si>
+    <t>Total Est. URA</t>
+  </si>
+  <si>
+    <t>WAC/Rx</t>
+  </si>
+  <si>
+    <t>Pharmacy Reimb/Rx</t>
+  </si>
+  <si>
+    <t>URA/Rx</t>
+  </si>
+  <si>
+    <t>Net Cost/Rx</t>
   </si>
   <si>
     <t>PDL Status</t>
@@ -265,12 +295,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="$#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,10 +356,10 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -335,21 +367,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,7 +411,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -421,7 +445,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -456,10 +479,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -632,21 +654,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Y54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="5" max="5" width="30.6640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="10.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="5" customWidth="1"/>
+    <col min="18" max="24" width="15.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="6" t="s">
         <v>66</v>
       </c>
@@ -686,8 +709,44 @@
       <c r="M1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="N1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -716,13 +775,31 @@
         <v>11</v>
       </c>
       <c r="K2" s="4">
-        <v>1.1270491803278691E-2</v>
+        <v>0.01127049180327869</v>
       </c>
       <c r="L2" s="5">
         <v>19276.45</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>2039.42</v>
+      </c>
+      <c r="N2">
+        <v>1946.08784</v>
+      </c>
+      <c r="O2">
+        <v>0.4886044028309997</v>
+      </c>
+      <c r="R2" s="5">
+        <v>22433.62</v>
+      </c>
+      <c r="S2" s="5">
+        <v>21406.96624</v>
+      </c>
+      <c r="T2" s="5">
+        <v>10961.16550343757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -751,13 +828,31 @@
         <v>18</v>
       </c>
       <c r="K3" s="4">
-        <v>1.8442622950819668E-2</v>
+        <v>0.01844262295081967</v>
       </c>
       <c r="L3" s="5">
         <v>31788.14</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>2039.42</v>
+      </c>
+      <c r="N3">
+        <v>1946.08784</v>
+      </c>
+      <c r="O3">
+        <v>0.4886044028309997</v>
+      </c>
+      <c r="R3" s="5">
+        <v>36709.56</v>
+      </c>
+      <c r="S3" s="5">
+        <v>35029.58112</v>
+      </c>
+      <c r="T3" s="5">
+        <v>17936.45264198875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -786,13 +881,31 @@
         <v>13</v>
       </c>
       <c r="K4" s="4">
-        <v>1.331967213114754E-2</v>
+        <v>0.01331967213114754</v>
       </c>
       <c r="L4" s="5">
         <v>24018.31</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>2039.42</v>
+      </c>
+      <c r="N4">
+        <v>1954.13866</v>
+      </c>
+      <c r="O4">
+        <v>0.5397648185489924</v>
+      </c>
+      <c r="R4" s="5">
+        <v>26512.46</v>
+      </c>
+      <c r="S4" s="5">
+        <v>25403.80258</v>
+      </c>
+      <c r="T4" s="5">
+        <v>14310.49316118742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -814,8 +927,17 @@
       <c r="G5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>2039.42</v>
+      </c>
+      <c r="N5">
+        <v>1954.13866</v>
+      </c>
+      <c r="O5">
+        <v>0.5397648185489924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -844,13 +966,31 @@
         <v>41</v>
       </c>
       <c r="K6" s="4">
-        <v>4.2008196721311467E-2</v>
+        <v>0.04200819672131147</v>
       </c>
       <c r="L6" s="5">
         <v>100464.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>2719.23</v>
+      </c>
+      <c r="N6">
+        <v>2603.06168</v>
+      </c>
+      <c r="O6">
+        <v>0.4886022626340079</v>
+      </c>
+      <c r="R6" s="5">
+        <v>111488.43</v>
+      </c>
+      <c r="S6" s="5">
+        <v>106725.52888</v>
+      </c>
+      <c r="T6" s="5">
+        <v>54473.49915551321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -879,13 +1019,31 @@
         <v>32</v>
       </c>
       <c r="K7" s="4">
-        <v>3.2786885245901641E-2</v>
+        <v>0.03278688524590164</v>
       </c>
       <c r="L7" s="5">
-        <v>78108.570000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>78108.57000000001</v>
+      </c>
+      <c r="M7">
+        <v>2719.23</v>
+      </c>
+      <c r="N7">
+        <v>2603.06168</v>
+      </c>
+      <c r="O7">
+        <v>0.4886022626340079</v>
+      </c>
+      <c r="R7" s="5">
+        <v>87015.36</v>
+      </c>
+      <c r="S7" s="5">
+        <v>83297.97375999999</v>
+      </c>
+      <c r="T7" s="5">
+        <v>42515.90177991275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -914,13 +1072,31 @@
         <v>18</v>
       </c>
       <c r="K8" s="4">
-        <v>1.8442622950819668E-2</v>
+        <v>0.01844262295081967</v>
       </c>
       <c r="L8" s="5">
         <v>40781.82</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>2719.23</v>
+      </c>
+      <c r="N8">
+        <v>2604.81627</v>
+      </c>
+      <c r="O8">
+        <v>0.5400719842236915</v>
+      </c>
+      <c r="R8" s="5">
+        <v>48946.14</v>
+      </c>
+      <c r="S8" s="5">
+        <v>46886.69286</v>
+      </c>
+      <c r="T8" s="5">
+        <v>26434.43894989059</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -949,13 +1125,31 @@
         <v>25</v>
       </c>
       <c r="K9" s="4">
-        <v>2.561475409836066E-2</v>
+        <v>0.02561475409836066</v>
       </c>
       <c r="L9" s="5">
         <v>58494.58</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>2719.23</v>
+      </c>
+      <c r="N9">
+        <v>2604.81627</v>
+      </c>
+      <c r="O9">
+        <v>0.5400719842236915</v>
+      </c>
+      <c r="R9" s="5">
+        <v>67980.75</v>
+      </c>
+      <c r="S9" s="5">
+        <v>65120.40674999999</v>
+      </c>
+      <c r="T9" s="5">
+        <v>36714.49854151472</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" outlineLevel="1">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -972,16 +1166,37 @@
         <v>1</v>
       </c>
       <c r="K10" s="4">
-        <v>0.16188524590163941</v>
+        <v>0.1618852459016394</v>
       </c>
       <c r="L10" s="5">
-        <v>352932.07000000012</v>
-      </c>
-      <c r="M10" t="s">
+        <v>352932.0700000001</v>
+      </c>
+      <c r="R10" s="5">
+        <v>401086.32</v>
+      </c>
+      <c r="S10" s="5">
+        <v>383870.95219</v>
+      </c>
+      <c r="T10" s="5">
+        <v>203346.449733445</v>
+      </c>
+      <c r="U10" s="5">
+        <v>2538.521012658228</v>
+      </c>
+      <c r="V10" s="5">
+        <v>2429.562988544304</v>
+      </c>
+      <c r="W10" s="5">
+        <v>1287.002846414209</v>
+      </c>
+      <c r="X10" s="5">
+        <v>1142.560142130095</v>
+      </c>
+      <c r="Y10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1003,8 +1218,17 @@
       <c r="G11">
         <v>2022</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>927.75897</v>
+      </c>
+      <c r="N11">
+        <v>885.8208</v>
+      </c>
+      <c r="O11">
+        <v>0.5400719842236915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1033,13 +1257,31 @@
         <v>15</v>
       </c>
       <c r="K12" s="4">
-        <v>1.536885245901639E-2</v>
+        <v>0.01536885245901639</v>
       </c>
       <c r="L12" s="5">
         <v>50424</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>927.75897</v>
+      </c>
+      <c r="N12">
+        <v>885.8208</v>
+      </c>
+      <c r="O12">
+        <v>0.5400719842236915</v>
+      </c>
+      <c r="R12" s="5">
+        <v>54273.899745</v>
+      </c>
+      <c r="S12" s="5">
+        <v>51820.5168</v>
+      </c>
+      <c r="T12" s="5">
+        <v>29311.81272683985</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1068,13 +1310,31 @@
         <v>28</v>
       </c>
       <c r="K13" s="4">
-        <v>2.8688524590163939E-2</v>
+        <v>0.02868852459016394</v>
       </c>
       <c r="L13" s="5">
         <v>38935.69</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>937.29375</v>
+      </c>
+      <c r="N13">
+        <v>897.30789</v>
+      </c>
+      <c r="O13">
+        <v>0.2718242193579422</v>
+      </c>
+      <c r="R13" s="5">
+        <v>41990.76</v>
+      </c>
+      <c r="S13" s="5">
+        <v>40199.393472</v>
+      </c>
+      <c r="T13" s="5">
+        <v>11414.10555724671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1103,13 +1363,31 @@
         <v>35</v>
       </c>
       <c r="K14" s="4">
-        <v>3.5860655737704923E-2</v>
+        <v>0.03586065573770492</v>
       </c>
       <c r="L14" s="5">
         <v>47531.83</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>937.29375</v>
+      </c>
+      <c r="N14">
+        <v>897.30789</v>
+      </c>
+      <c r="O14">
+        <v>0.2718242193579422</v>
+      </c>
+      <c r="R14" s="5">
+        <v>52488.45</v>
+      </c>
+      <c r="S14" s="5">
+        <v>50249.24184</v>
+      </c>
+      <c r="T14" s="5">
+        <v>14267.63194655838</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1138,13 +1416,31 @@
         <v>27</v>
       </c>
       <c r="K15" s="4">
-        <v>2.7663934426229511E-2</v>
+        <v>0.02766393442622951</v>
       </c>
       <c r="L15" s="5">
         <v>53544.86</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>938.00416</v>
+      </c>
+      <c r="N15">
+        <v>896.90851</v>
+      </c>
+      <c r="O15">
+        <v>0.2733784107296016</v>
+      </c>
+      <c r="R15" s="5">
+        <v>60782.669568</v>
+      </c>
+      <c r="S15" s="5">
+        <v>58119.67144799999</v>
+      </c>
+      <c r="T15" s="5">
+        <v>16616.66960640236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1173,13 +1469,31 @@
         <v>22</v>
       </c>
       <c r="K16" s="4">
-        <v>2.2540983606557381E-2</v>
+        <v>0.02254098360655738</v>
       </c>
       <c r="L16" s="5">
         <v>43952.88</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>938.00416</v>
+      </c>
+      <c r="N16">
+        <v>896.90851</v>
+      </c>
+      <c r="O16">
+        <v>0.2733784107296016</v>
+      </c>
+      <c r="R16" s="5">
+        <v>49526.61964799999</v>
+      </c>
+      <c r="S16" s="5">
+        <v>47356.76932799999</v>
+      </c>
+      <c r="T16" s="5">
+        <v>13539.5085681797</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1208,13 +1522,31 @@
         <v>32</v>
       </c>
       <c r="K17" s="4">
-        <v>3.2786885245901641E-2</v>
+        <v>0.03278688524590164</v>
       </c>
       <c r="L17" s="5">
-        <v>86742.04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>86742.03999999999</v>
+      </c>
+      <c r="M17">
+        <v>937.29062</v>
+      </c>
+      <c r="N17">
+        <v>897.1534</v>
+      </c>
+      <c r="O17">
+        <v>0.2759222965803138</v>
+      </c>
+      <c r="R17" s="5">
+        <v>95978.559488</v>
+      </c>
+      <c r="S17" s="5">
+        <v>91868.50816000001</v>
+      </c>
+      <c r="T17" s="5">
+        <v>26482.62455639923</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1243,13 +1575,31 @@
         <v>31</v>
       </c>
       <c r="K18" s="4">
-        <v>3.1762295081967207E-2</v>
+        <v>0.03176229508196721</v>
       </c>
       <c r="L18" s="5">
         <v>84826.91</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>937.29062</v>
+      </c>
+      <c r="N18">
+        <v>897.1534</v>
+      </c>
+      <c r="O18">
+        <v>0.2759222965803138</v>
+      </c>
+      <c r="R18" s="5">
+        <v>92979.229504</v>
+      </c>
+      <c r="S18" s="5">
+        <v>88997.61728000001</v>
+      </c>
+      <c r="T18" s="5">
+        <v>25655.04253901175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1271,8 +1621,14 @@
       <c r="G19">
         <v>2022</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>956.425</v>
+      </c>
+      <c r="O19">
+        <v>0.231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1294,8 +1650,14 @@
       <c r="G20">
         <v>2022</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>956.425</v>
+      </c>
+      <c r="O20">
+        <v>0.231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" outlineLevel="1">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -1303,25 +1665,46 @@
         <v>24</v>
       </c>
       <c r="H21" s="2">
-        <v>478.50000000000011</v>
+        <v>478.5000000000001</v>
       </c>
       <c r="I21" s="2">
         <v>190</v>
       </c>
       <c r="J21" s="3">
-        <v>2.5184210526315791</v>
+        <v>2.518421052631579</v>
       </c>
       <c r="K21" s="4">
-        <v>0.19467213114754101</v>
+        <v>0.194672131147541</v>
       </c>
       <c r="L21" s="5">
         <v>405958.21</v>
       </c>
-      <c r="M21" t="s">
+      <c r="R21" s="5">
+        <v>448020.187953</v>
+      </c>
+      <c r="S21" s="5">
+        <v>428611.718328</v>
+      </c>
+      <c r="T21" s="5">
+        <v>137287.395500638</v>
+      </c>
+      <c r="U21" s="5">
+        <v>2358.000989226316</v>
+      </c>
+      <c r="V21" s="5">
+        <v>2255.851149094737</v>
+      </c>
+      <c r="W21" s="5">
+        <v>722.5652394770419</v>
+      </c>
+      <c r="X21" s="5">
+        <v>1533.285909617695</v>
+      </c>
+      <c r="Y21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1343,8 +1726,14 @@
       <c r="G22">
         <v>2022</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>3983.282</v>
+      </c>
+      <c r="O22">
+        <v>0.231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" outlineLevel="1">
       <c r="B23" t="s">
         <v>1</v>
       </c>
@@ -1366,11 +1755,32 @@
       <c r="L23" s="5">
         <v>0</v>
       </c>
-      <c r="M23" t="s">
+      <c r="R23" s="5">
+        <v>0</v>
+      </c>
+      <c r="S23" s="5">
+        <v>0</v>
+      </c>
+      <c r="T23" s="5">
+        <v>0</v>
+      </c>
+      <c r="U23" s="5">
+        <v>0</v>
+      </c>
+      <c r="V23" s="5">
+        <v>0</v>
+      </c>
+      <c r="W23" s="5">
+        <v>0</v>
+      </c>
+      <c r="X23" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1399,13 +1809,31 @@
         <v>20</v>
       </c>
       <c r="K24" s="4">
-        <v>2.049180327868852E-2</v>
+        <v>0.02049180327868852</v>
       </c>
       <c r="L24" s="5">
         <v>28183.19</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>2232.05333</v>
+      </c>
+      <c r="N24">
+        <v>2146.43636</v>
+      </c>
+      <c r="O24">
+        <v>0.6101297289535604</v>
+      </c>
+      <c r="R24" s="5">
+        <v>33480.79995</v>
+      </c>
+      <c r="S24" s="5">
+        <v>32196.5454</v>
+      </c>
+      <c r="T24" s="5">
+        <v>20427.63139864188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1434,13 +1862,31 @@
         <v>28</v>
       </c>
       <c r="K25" s="4">
-        <v>2.8688524590163939E-2</v>
+        <v>0.02868852459016394</v>
       </c>
       <c r="L25" s="5">
-        <v>41537.919999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>41537.92</v>
+      </c>
+      <c r="M25">
+        <v>2232.05333</v>
+      </c>
+      <c r="N25">
+        <v>2146.43636</v>
+      </c>
+      <c r="O25">
+        <v>0.6101297289535604</v>
+      </c>
+      <c r="R25" s="5">
+        <v>48547.1599275</v>
+      </c>
+      <c r="S25" s="5">
+        <v>46684.99083</v>
+      </c>
+      <c r="T25" s="5">
+        <v>29620.06552803073</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1469,13 +1915,31 @@
         <v>67</v>
       </c>
       <c r="K26" s="4">
-        <v>6.8647540983606564E-2</v>
+        <v>0.06864754098360656</v>
       </c>
       <c r="L26" s="5">
         <v>130785.82</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>2232.14</v>
+      </c>
+      <c r="N26">
+        <v>2151.01264</v>
+      </c>
+      <c r="O26">
+        <v>0.610132770470352</v>
+      </c>
+      <c r="R26" s="5">
+        <v>151785.52</v>
+      </c>
+      <c r="S26" s="5">
+        <v>146268.85952</v>
+      </c>
+      <c r="T26" s="5">
+        <v>92609.31983488302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1504,13 +1968,31 @@
         <v>69</v>
       </c>
       <c r="K27" s="4">
-        <v>7.0696721311475405E-2</v>
+        <v>0.07069672131147541</v>
       </c>
       <c r="L27" s="5">
-        <v>135153.17000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>135153.17</v>
+      </c>
+      <c r="M27">
+        <v>2232.14</v>
+      </c>
+      <c r="N27">
+        <v>2151.01264</v>
+      </c>
+      <c r="O27">
+        <v>0.610132770470352</v>
+      </c>
+      <c r="R27" s="5">
+        <v>154017.66</v>
+      </c>
+      <c r="S27" s="5">
+        <v>148419.87216</v>
+      </c>
+      <c r="T27" s="5">
+        <v>93971.22159716071</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1539,13 +2021,31 @@
         <v>102</v>
       </c>
       <c r="K28" s="4">
-        <v>0.10450819672131149</v>
+        <v>0.1045081967213115</v>
       </c>
       <c r="L28" s="5">
-        <v>291004.78000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>291004.78</v>
+      </c>
+      <c r="M28">
+        <v>2232.08</v>
+      </c>
+      <c r="N28">
+        <v>2146.93494</v>
+      </c>
+      <c r="O28">
+        <v>0.6101167428934857</v>
+      </c>
+      <c r="R28" s="5">
+        <v>341508.24</v>
+      </c>
+      <c r="S28" s="5">
+        <v>328481.04582</v>
+      </c>
+      <c r="T28" s="5">
+        <v>208359.8950600868</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1579,8 +2079,26 @@
       <c r="L29" s="5">
         <v>311818.42</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>2232.08</v>
+      </c>
+      <c r="N29">
+        <v>2146.93494</v>
+      </c>
+      <c r="O29">
+        <v>0.6101167428934857</v>
+      </c>
+      <c r="R29" s="5">
+        <v>354900.72</v>
+      </c>
+      <c r="S29" s="5">
+        <v>341362.65546</v>
+      </c>
+      <c r="T29" s="5">
+        <v>216530.871336953</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1602,8 +2120,17 @@
       <c r="G30">
         <v>2022</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>2231.92</v>
+      </c>
+      <c r="N30">
+        <v>1714.79519</v>
+      </c>
+      <c r="O30">
+        <v>0.6101102033288768</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1625,8 +2152,17 @@
       <c r="G31">
         <v>2022</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <v>2231.92</v>
+      </c>
+      <c r="N31">
+        <v>1714.79519</v>
+      </c>
+      <c r="O31">
+        <v>0.6101102033288768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1648,8 +2184,17 @@
       <c r="G32">
         <v>2022</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>2232.02</v>
+      </c>
+      <c r="N32">
+        <v>2142.05707</v>
+      </c>
+      <c r="O32">
+        <v>0.6101127821986614</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" outlineLevel="1">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -1663,19 +2208,40 @@
         <v>392</v>
       </c>
       <c r="J33" s="3">
-        <v>1.2391581632653059</v>
+        <v>1.239158163265306</v>
       </c>
       <c r="K33" s="4">
-        <v>0.40163934426229508</v>
+        <v>0.4016393442622951</v>
       </c>
       <c r="L33" s="5">
-        <v>938483.29999999993</v>
-      </c>
-      <c r="M33" t="s">
+        <v>938483.2999999999</v>
+      </c>
+      <c r="R33" s="5">
+        <v>1084240.0998775</v>
+      </c>
+      <c r="S33" s="5">
+        <v>1043413.96919</v>
+      </c>
+      <c r="T33" s="5">
+        <v>661519.0047557561</v>
+      </c>
+      <c r="U33" s="5">
+        <v>2765.918622136479</v>
+      </c>
+      <c r="V33" s="5">
+        <v>2661.770329566326</v>
+      </c>
+      <c r="W33" s="5">
+        <v>1687.548481519786</v>
+      </c>
+      <c r="X33" s="5">
+        <v>974.2218480465403</v>
+      </c>
+      <c r="Y33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1697,8 +2263,14 @@
       <c r="G34">
         <v>2022</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>3804.56818</v>
+      </c>
+      <c r="O34">
+        <v>0.4706464368934038</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1720,8 +2292,17 @@
       <c r="G35">
         <v>2022</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>3804.62879</v>
+      </c>
+      <c r="N35">
+        <v>3603.46281</v>
+      </c>
+      <c r="O35">
+        <v>0.4720617423978541</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1743,8 +2324,17 @@
       <c r="G36">
         <v>2022</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <v>3804.62879</v>
+      </c>
+      <c r="N36">
+        <v>3603.46281</v>
+      </c>
+      <c r="O36">
+        <v>0.4720617423978541</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1773,13 +2363,31 @@
         <v>11</v>
       </c>
       <c r="K37" s="4">
-        <v>1.1270491803278691E-2</v>
+        <v>0.01127049180327869</v>
       </c>
       <c r="L37" s="5">
         <v>62236.06</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>3826.52</v>
+      </c>
+      <c r="N37">
+        <v>3658.46827</v>
+      </c>
+      <c r="O37">
+        <v>0.4748453212646796</v>
+      </c>
+      <c r="R37" s="5">
+        <v>73660.50999999999</v>
+      </c>
+      <c r="S37" s="5">
+        <v>70425.5141975</v>
+      </c>
+      <c r="T37" s="5">
+        <v>34977.34853547014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1801,8 +2409,17 @@
       <c r="G38">
         <v>2022</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>3826.52</v>
+      </c>
+      <c r="N38">
+        <v>3658.46827</v>
+      </c>
+      <c r="O38">
+        <v>0.4748453212646796</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1831,13 +2448,31 @@
         <v>15</v>
       </c>
       <c r="K39" s="4">
-        <v>1.536885245901639E-2</v>
+        <v>0.01536885245901639</v>
       </c>
       <c r="L39" s="5">
         <v>127751.19</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <v>3819.15589</v>
+      </c>
+      <c r="N39">
+        <v>3668.26596</v>
+      </c>
+      <c r="O39">
+        <v>0.4734493612902498</v>
+      </c>
+      <c r="R39" s="5">
+        <v>150551.1251838</v>
+      </c>
+      <c r="S39" s="5">
+        <v>144603.0441432</v>
+      </c>
+      <c r="T39" s="5">
+        <v>71278.33405979855</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1866,13 +2501,31 @@
         <v>17</v>
       </c>
       <c r="K40" s="4">
-        <v>1.7418032786885241E-2</v>
+        <v>0.01741803278688524</v>
       </c>
       <c r="L40" s="5">
         <v>150064.93</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="M40">
+        <v>3819.15589</v>
+      </c>
+      <c r="N40">
+        <v>3668.26596</v>
+      </c>
+      <c r="O40">
+        <v>0.4734493612902498</v>
+      </c>
+      <c r="R40" s="5">
+        <v>170639.8851652</v>
+      </c>
+      <c r="S40" s="5">
+        <v>163898.1230928</v>
+      </c>
+      <c r="T40" s="5">
+        <v>80789.3446421055</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" outlineLevel="1">
       <c r="B41" t="s">
         <v>1</v>
       </c>
@@ -1886,19 +2539,40 @@
         <v>43</v>
       </c>
       <c r="J41" s="3">
-        <v>2.4034883720930229</v>
+        <v>2.403488372093023</v>
       </c>
       <c r="K41" s="4">
-        <v>4.4057377049180328E-2</v>
+        <v>0.04405737704918033</v>
       </c>
       <c r="L41" s="5">
         <v>340052.18</v>
       </c>
-      <c r="M41" t="s">
+      <c r="R41" s="5">
+        <v>394851.520349</v>
+      </c>
+      <c r="S41" s="5">
+        <v>378926.6814335</v>
+      </c>
+      <c r="T41" s="5">
+        <v>187045.0272373742</v>
+      </c>
+      <c r="U41" s="5">
+        <v>9182.593496488373</v>
+      </c>
+      <c r="V41" s="5">
+        <v>8812.248405430233</v>
+      </c>
+      <c r="W41" s="5">
+        <v>4349.884354357539</v>
+      </c>
+      <c r="X41" s="5">
+        <v>4462.364051072694</v>
+      </c>
+      <c r="Y41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1920,8 +2594,17 @@
       <c r="G42">
         <v>2022</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <v>2070.59</v>
+      </c>
+      <c r="N42">
+        <v>1966.31473</v>
+      </c>
+      <c r="O42">
+        <v>0.2548310605489526</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" outlineLevel="1">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -1943,11 +2626,32 @@
       <c r="L43" s="5">
         <v>0</v>
       </c>
-      <c r="M43" t="s">
+      <c r="R43" s="5">
+        <v>0</v>
+      </c>
+      <c r="S43" s="5">
+        <v>0</v>
+      </c>
+      <c r="T43" s="5">
+        <v>0</v>
+      </c>
+      <c r="U43" s="5">
+        <v>0</v>
+      </c>
+      <c r="V43" s="5">
+        <v>0</v>
+      </c>
+      <c r="W43" s="5">
+        <v>0</v>
+      </c>
+      <c r="X43" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1969,8 +2673,17 @@
       <c r="G44">
         <v>2022</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <v>293.23</v>
+      </c>
+      <c r="N44">
+        <v>281.27964</v>
+      </c>
+      <c r="O44">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1992,8 +2705,17 @@
       <c r="G45">
         <v>2022</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M45">
+        <v>293.23</v>
+      </c>
+      <c r="N45">
+        <v>281.27964</v>
+      </c>
+      <c r="O45">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2015,8 +2737,17 @@
       <c r="G46">
         <v>2022</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M46">
+        <v>586.41</v>
+      </c>
+      <c r="N46">
+        <v>562.0587</v>
+      </c>
+      <c r="O46">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2038,8 +2769,17 @@
       <c r="G47">
         <v>2022</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M47">
+        <v>586.41</v>
+      </c>
+      <c r="N47">
+        <v>562.0587</v>
+      </c>
+      <c r="O47">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2068,13 +2808,31 @@
         <v>30</v>
       </c>
       <c r="K48" s="4">
-        <v>3.073770491803279E-2</v>
+        <v>0.03073770491803279</v>
       </c>
       <c r="L48" s="5">
         <v>25305.98</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M48">
+        <v>879.66</v>
+      </c>
+      <c r="N48">
+        <v>842.62657</v>
+      </c>
+      <c r="O48">
+        <v>0.7</v>
+      </c>
+      <c r="R48" s="5">
+        <v>29028.78</v>
+      </c>
+      <c r="S48" s="5">
+        <v>27806.67681</v>
+      </c>
+      <c r="T48" s="5">
+        <v>20320.146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2103,13 +2861,31 @@
         <v>19</v>
       </c>
       <c r="K49" s="4">
-        <v>1.9467213114754099E-2</v>
+        <v>0.0194672131147541</v>
       </c>
       <c r="L49" s="5">
         <v>17791.68</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M49">
+        <v>879.66</v>
+      </c>
+      <c r="N49">
+        <v>842.62657</v>
+      </c>
+      <c r="O49">
+        <v>0.7</v>
+      </c>
+      <c r="R49" s="5">
+        <v>20232.18</v>
+      </c>
+      <c r="S49" s="5">
+        <v>19380.41111</v>
+      </c>
+      <c r="T49" s="5">
+        <v>14162.526</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2138,13 +2914,31 @@
         <v>75</v>
       </c>
       <c r="K50" s="4">
-        <v>7.6844262295081969E-2</v>
+        <v>0.07684426229508197</v>
       </c>
       <c r="L50" s="5">
         <v>80435.75</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="M50">
+        <v>1172.91</v>
+      </c>
+      <c r="N50">
+        <v>1124.80239</v>
+      </c>
+      <c r="O50">
+        <v>0.7</v>
+      </c>
+      <c r="R50" s="5">
+        <v>96178.62000000001</v>
+      </c>
+      <c r="S50" s="5">
+        <v>92233.79598000001</v>
+      </c>
+      <c r="T50" s="5">
+        <v>67325.034</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" hidden="1" outlineLevel="2">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2173,13 +2967,31 @@
         <v>69</v>
       </c>
       <c r="K51" s="4">
-        <v>7.0696721311475405E-2</v>
+        <v>0.07069672131147541</v>
       </c>
       <c r="L51" s="5">
-        <v>79281.179999999993</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+        <v>79281.17999999999</v>
+      </c>
+      <c r="M51">
+        <v>1172.91</v>
+      </c>
+      <c r="N51">
+        <v>1124.80239</v>
+      </c>
+      <c r="O51">
+        <v>0.7</v>
+      </c>
+      <c r="R51" s="5">
+        <v>95005.71000000001</v>
+      </c>
+      <c r="S51" s="5">
+        <v>91108.99359</v>
+      </c>
+      <c r="T51" s="5">
+        <v>66503.997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" outlineLevel="1">
       <c r="B52" t="s">
         <v>1</v>
       </c>
@@ -2201,11 +3013,32 @@
       <c r="L52" s="5">
         <v>202814.59</v>
       </c>
-      <c r="M52" t="s">
+      <c r="R52" s="5">
+        <v>240445.29</v>
+      </c>
+      <c r="S52" s="5">
+        <v>230529.87749</v>
+      </c>
+      <c r="T52" s="5">
+        <v>168311.703</v>
+      </c>
+      <c r="U52" s="5">
+        <v>1245.830518134715</v>
+      </c>
+      <c r="V52" s="5">
+        <v>1194.455323782384</v>
+      </c>
+      <c r="W52" s="5">
+        <v>872.0813626943005</v>
+      </c>
+      <c r="X52" s="5">
+        <v>322.3739610880831</v>
+      </c>
+      <c r="Y52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" outlineLevel="1">
       <c r="B53" t="s">
         <v>65</v>
       </c>
@@ -2218,10 +3051,19 @@
       <c r="L53" s="5">
         <v>2240240.35</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R53" s="5">
+        <v>2568643.4181795</v>
+      </c>
+      <c r="S53" s="5">
+        <v>2465353.1986315</v>
+      </c>
+      <c r="T53" s="5">
+        <v>1357509.580227213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
       <c r="E54" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H54" s="2">
         <v>1444.6</v>
@@ -2231,6 +3073,15 @@
       </c>
       <c r="L54" s="5">
         <v>2240240.35</v>
+      </c>
+      <c r="R54" s="5">
+        <v>2568643.4181795</v>
+      </c>
+      <c r="S54" s="5">
+        <v>2465353.1986315</v>
+      </c>
+      <c r="T54" s="5">
+        <v>1357509.580227213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>